<commit_message>
Apparently I made a change to this spreadsheet
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0FB178-AD32-43A6-9B69-B4FFC313D940}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5824550E-C948-494C-9FFC-E9C465E68573}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF99BAD5-59DB-4CD8-989F-B83D7F3C1D42}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Got pretty much same results after changing Tarrival initial condition
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5824550E-C948-494C-9FFC-E9C465E68573}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52B6443-1462-48D1-B1C1-4BA8AFB2D1A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF99BAD5-59DB-4CD8-989F-B83D7F3C1D42}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Rmse parameter to running multiple files script and changed up spreadsheet a bit so that it wouldn't affect it
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B396024-7C12-4DC6-A29C-8164A338E4F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50997F2E-33F7-41D4-876E-85896CBB02B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,13 +123,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -450,7 +458,7 @@
   <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M16"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,39 +671,39 @@
       <c r="M5">
         <v>0.98797313519992624</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f>0.0001</f>
         <v>1E-4</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>1E-4</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <f>1/38</f>
         <v>2.6315789473684209E-2</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f>10^8</f>
         <v>100000000</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>20</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>40</v>
-      </c>
-      <c r="V5">
-        <f>0.00000001</f>
-        <v>1E-8</v>
       </c>
       <c r="W5">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="X5">
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="Y5">
         <v>0</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>0</v>
       </c>
     </row>
@@ -739,37 +747,37 @@
       <c r="M6">
         <v>0.96261722780743508</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.08</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>10</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f>10^100</f>
         <v>1E+100</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>60</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <f>10^100</f>
         <v>1E+100</v>
       </c>
-      <c r="V6">
-        <v>10</v>
-      </c>
       <c r="W6">
         <v>10</v>
       </c>
       <c r="X6">
+        <v>10</v>
+      </c>
+      <c r="Y6">
         <v>0.9</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>0.1</v>
       </c>
     </row>
@@ -1182,45 +1190,6 @@
       <c r="M16">
         <v>0.89643729705960273</v>
       </c>
-      <c r="N16" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P16" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>3</v>
-      </c>
-      <c r="R16" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16" t="s">
-        <v>5</v>
-      </c>
-      <c r="T16" t="s">
-        <v>9</v>
-      </c>
-      <c r="U16" t="s">
-        <v>10</v>
-      </c>
-      <c r="V16" t="s">
-        <v>11</v>
-      </c>
-      <c r="W16" t="s">
-        <v>12</v>
-      </c>
-      <c r="X16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
@@ -1236,57 +1205,48 @@
         <v>16</v>
       </c>
       <c r="N17" t="str">
-        <f>_xlfn.IFS(ABS(A1-P$5)&lt;=0.01*P$5,"Lower",ABS(A1-P$6)&lt;=0.01*P$6,"Upper",TRUE,"Ok")</f>
+        <f>_xlfn.IFS(ABS(A1-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A1-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" ref="O17:Z32" si="0">_xlfn.IFS(ABS(B1-Q$5)&lt;=0.01*Q$5,"Lower",ABS(B1-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
+        <f>_xlfn.IFS(ABS(B1-R$5)&lt;=0.01*R$5,"Lower",ABS(B1-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C1-S$5)&lt;=0.01*S$5,"Lower",ABS(C1-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D1-T$5)&lt;=0.01*T$5,"Lower",ABS(D1-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E1-U$5)&lt;=0.01*U$5,"Lower",ABS(E1-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F1-V$5)&lt;=0.01*V$5,"Lower",ABS(F1-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G1-W$5)&lt;=0.01*W$5,"Lower",ABS(G1-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H1-X$5)&lt;=0.01*X$5,"Lower",ABS(H1-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V17" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I1-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I1-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X17" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y17" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z17" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J1-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J1-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1309,57 +1269,48 @@
         <v>1.8622126579096846E-2</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" ref="N18:N32" si="1">_xlfn.IFS(ABS(A2-P$5)&lt;=0.01*P$5,"Lower",ABS(A2-P$6)&lt;=0.01*P$6,"Upper",TRUE,"Ok")</f>
+        <f>_xlfn.IFS(ABS(A2-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A2-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B2-R$5)&lt;=0.01*R$5,"Lower",ABS(B2-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C2-S$5)&lt;=0.01*S$5,"Lower",ABS(C2-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D2-T$5)&lt;=0.01*T$5,"Lower",ABS(D2-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E2-U$5)&lt;=0.01*U$5,"Lower",ABS(E2-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F2-V$5)&lt;=0.01*V$5,"Lower",ABS(F2-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G2-W$5)&lt;=0.01*W$5,"Lower",ABS(G2-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H2-X$5)&lt;=0.01*X$5,"Lower",ABS(H2-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I2-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I2-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X18" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y18" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z18" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J2-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J2-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B19">
@@ -1379,111 +1330,93 @@
         <v>3.6968551269839821E-3</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A3-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A3-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B3-R$5)&lt;=0.01*R$5,"Lower",ABS(B3-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C3-S$5)&lt;=0.01*S$5,"Lower",ABS(C3-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D3-T$5)&lt;=0.01*T$5,"Lower",ABS(D3-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E3-U$5)&lt;=0.01*U$5,"Lower",ABS(E3-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F3-V$5)&lt;=0.01*V$5,"Lower",ABS(F3-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G3-W$5)&lt;=0.01*W$5,"Lower",ABS(G3-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H3-X$5)&lt;=0.01*X$5,"Lower",ABS(H3-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V19" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I3-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I3-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X19" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y19" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z19" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J3-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J3-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A4-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A4-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B4-R$5)&lt;=0.01*R$5,"Lower",ABS(B4-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C4-S$5)&lt;=0.01*S$5,"Lower",ABS(C4-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D4-T$5)&lt;=0.01*T$5,"Lower",ABS(D4-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E4-U$5)&lt;=0.01*U$5,"Lower",ABS(E4-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F4-V$5)&lt;=0.01*V$5,"Lower",ABS(F4-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G4-W$5)&lt;=0.01*W$5,"Lower",ABS(G4-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H4-X$5)&lt;=0.01*X$5,"Lower",ABS(H4-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I4-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I4-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X20" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y20" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z20" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J4-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J4-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
@@ -1499,57 +1432,48 @@
         <v>16</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A5-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A5-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B5-R$5)&lt;=0.01*R$5,"Lower",ABS(B5-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C5-S$5)&lt;=0.01*S$5,"Lower",ABS(C5-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D5-T$5)&lt;=0.01*T$5,"Lower",ABS(D5-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E5-U$5)&lt;=0.01*U$5,"Lower",ABS(E5-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F5-V$5)&lt;=0.01*V$5,"Lower",ABS(F5-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G5-W$5)&lt;=0.01*W$5,"Lower",ABS(G5-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H5-X$5)&lt;=0.01*X$5,"Lower",ABS(H5-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I5-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I5-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X21" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y21" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z21" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J5-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J5-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
@@ -1572,57 +1496,48 @@
         <v>0.59155156721494173</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A6-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A6-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B6-R$5)&lt;=0.01*R$5,"Lower",ABS(B6-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C6-S$5)&lt;=0.01*S$5,"Lower",ABS(C6-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D6-T$5)&lt;=0.01*T$5,"Lower",ABS(D6-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E6-U$5)&lt;=0.01*U$5,"Lower",ABS(E6-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F6-V$5)&lt;=0.01*V$5,"Lower",ABS(F6-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G6-W$5)&lt;=0.01*W$5,"Lower",ABS(G6-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H6-X$5)&lt;=0.01*X$5,"Lower",ABS(H6-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V22" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I6-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I6-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X22" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y22" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z22" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J6-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J6-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C23">
@@ -1642,111 +1557,93 @@
         <v>0.21521679706093569</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A7-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A7-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B7-R$5)&lt;=0.01*R$5,"Lower",ABS(B7-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C7-S$5)&lt;=0.01*S$5,"Lower",ABS(C7-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D7-T$5)&lt;=0.01*T$5,"Lower",ABS(D7-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E7-U$5)&lt;=0.01*U$5,"Lower",ABS(E7-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F7-V$5)&lt;=0.01*V$5,"Lower",ABS(F7-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G7-W$5)&lt;=0.01*W$5,"Lower",ABS(G7-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H7-X$5)&lt;=0.01*X$5,"Lower",ABS(H7-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V23" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I7-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I7-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Upper</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X23" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y23" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z23" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J7-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J7-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N24" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A8-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A8-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B8-R$5)&lt;=0.01*R$5,"Lower",ABS(B8-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C8-S$5)&lt;=0.01*S$5,"Lower",ABS(C8-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D8-T$5)&lt;=0.01*T$5,"Lower",ABS(D8-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E8-U$5)&lt;=0.01*U$5,"Lower",ABS(E8-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F8-V$5)&lt;=0.01*V$5,"Lower",ABS(F8-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G8-W$5)&lt;=0.01*W$5,"Lower",ABS(G8-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H8-X$5)&lt;=0.01*X$5,"Lower",ABS(H8-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V24" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I8-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I8-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X24" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y24" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z24" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J8-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J8-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
@@ -1762,57 +1659,48 @@
         <v>16</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A9-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A9-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B9-R$5)&lt;=0.01*R$5,"Lower",ABS(B9-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C9-S$5)&lt;=0.01*S$5,"Lower",ABS(C9-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D9-T$5)&lt;=0.01*T$5,"Lower",ABS(D9-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E9-U$5)&lt;=0.01*U$5,"Lower",ABS(E9-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F9-V$5)&lt;=0.01*V$5,"Lower",ABS(F9-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G9-W$5)&lt;=0.01*W$5,"Lower",ABS(G9-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H9-X$5)&lt;=0.01*X$5,"Lower",ABS(H9-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V25" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I9-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I9-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X25" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y25" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z25" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J9-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J9-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
@@ -1835,57 +1723,48 @@
         <v>4.6496103808292069E-2</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A10-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A10-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B10-R$5)&lt;=0.01*R$5,"Lower",ABS(B10-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C10-S$5)&lt;=0.01*S$5,"Lower",ABS(C10-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D10-T$5)&lt;=0.01*T$5,"Lower",ABS(D10-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E10-U$5)&lt;=0.01*U$5,"Lower",ABS(E10-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F10-V$5)&lt;=0.01*V$5,"Lower",ABS(F10-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G10-W$5)&lt;=0.01*W$5,"Lower",ABS(G10-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H10-X$5)&lt;=0.01*X$5,"Lower",ABS(H10-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V26" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I10-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I10-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X26" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y26" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z26" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J10-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J10-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D27">
@@ -1905,111 +1784,93 @@
         <v>1.1591637186701999E-2</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A11-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A11-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B11-R$5)&lt;=0.01*R$5,"Lower",ABS(B11-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C11-S$5)&lt;=0.01*S$5,"Lower",ABS(C11-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D11-T$5)&lt;=0.01*T$5,"Lower",ABS(D11-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E11-U$5)&lt;=0.01*U$5,"Lower",ABS(E11-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F11-V$5)&lt;=0.01*V$5,"Lower",ABS(F11-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G11-W$5)&lt;=0.01*W$5,"Lower",ABS(G11-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Upper</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H11-X$5)&lt;=0.01*X$5,"Lower",ABS(H11-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V27" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I11-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I11-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W27" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X27" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y27" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z27" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J11-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J11-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N28" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A12-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A12-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B12-R$5)&lt;=0.01*R$5,"Lower",ABS(B12-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C12-S$5)&lt;=0.01*S$5,"Lower",ABS(C12-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D12-T$5)&lt;=0.01*T$5,"Lower",ABS(D12-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E12-U$5)&lt;=0.01*U$5,"Lower",ABS(E12-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Lower</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F12-V$5)&lt;=0.01*V$5,"Lower",ABS(F12-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G12-W$5)&lt;=0.01*W$5,"Lower",ABS(G12-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H12-X$5)&lt;=0.01*X$5,"Lower",ABS(H12-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V28" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I12-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I12-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W28" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X28" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y28" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z28" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J12-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J12-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
@@ -2025,57 +1886,48 @@
         <v>16</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A13-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A13-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B13-R$5)&lt;=0.01*R$5,"Lower",ABS(B13-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C13-S$5)&lt;=0.01*S$5,"Lower",ABS(C13-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D13-T$5)&lt;=0.01*T$5,"Lower",ABS(D13-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E13-U$5)&lt;=0.01*U$5,"Lower",ABS(E13-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F13-V$5)&lt;=0.01*V$5,"Lower",ABS(F13-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G13-W$5)&lt;=0.01*W$5,"Lower",ABS(G13-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H13-X$5)&lt;=0.01*X$5,"Lower",ABS(H13-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V29" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I13-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I13-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W29" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X29" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y29" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z29" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J13-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J13-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
@@ -2098,57 +1950,48 @@
         <v>874960948.85297513</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A14-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A14-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B14-R$5)&lt;=0.01*R$5,"Lower",ABS(B14-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C14-S$5)&lt;=0.01*S$5,"Lower",ABS(C14-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D14-T$5)&lt;=0.01*T$5,"Lower",ABS(D14-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E14-U$5)&lt;=0.01*U$5,"Lower",ABS(E14-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F14-V$5)&lt;=0.01*V$5,"Lower",ABS(F14-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G14-W$5)&lt;=0.01*W$5,"Lower",ABS(G14-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H14-X$5)&lt;=0.01*X$5,"Lower",ABS(H14-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V30" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I14-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I14-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X30" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y30" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z30" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J14-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J14-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E31">
@@ -2168,113 +2011,95 @@
         <v>135273086.9832198</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A15-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A15-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B15-R$5)&lt;=0.01*R$5,"Lower",ABS(B15-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C15-S$5)&lt;=0.01*S$5,"Lower",ABS(C15-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D15-T$5)&lt;=0.01*T$5,"Lower",ABS(D15-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E15-U$5)&lt;=0.01*U$5,"Lower",ABS(E15-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F15-V$5)&lt;=0.01*V$5,"Lower",ABS(F15-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G15-W$5)&lt;=0.01*W$5,"Lower",ABS(G15-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H15-X$5)&lt;=0.01*X$5,"Lower",ABS(H15-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V31" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I15-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I15-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X31" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y31" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z31" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
+        <f>_xlfn.IFS(ABS(J15-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J15-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N32" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.IFS(ABS(A16-Q$5)&lt;=0.01*Q$5,"Lower",ABS(A16-Q$6)&lt;=0.01*Q$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(B16-R$5)&lt;=0.01*R$5,"Lower",ABS(B16-R$6)&lt;=0.01*R$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C16-S$5)&lt;=0.01*S$5,"Lower",ABS(C16-S$6)&lt;=0.01*S$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(D16-T$5)&lt;=0.01*T$5,"Lower",ABS(D16-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E16-U$5)&lt;=0.01*U$5,"Lower",ABS(E16-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F16-V$5)&lt;=0.01*V$5,"Lower",ABS(F16-V$6)&lt;=0.01*V$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(G16-W$5)&lt;=0.01*W$5,"Lower",ABS(G16-W$6)&lt;=0.01*W$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H16-X$5)&lt;=0.01*X$5,"Lower",ABS(H16-X$6)&lt;=0.01*X$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="V32" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(I16-Y$5)&lt;=0.01*Y$5,"Lower",ABS(I16-Y$6)&lt;=0.01*Y$6,"Upper",TRUE,"Ok")</f>
         <v>Ok</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="X32" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Y32" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-      <c r="Z32" t="str">
-        <f t="shared" si="0"/>
-        <v>Ok</v>
-      </c>
-    </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.3">
+        <f>_xlfn.IFS(ABS(J16-Z$5)&lt;=0.01*Z$5,"Lower",ABS(J16-Z$6)&lt;=0.01*Z$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="5:26" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>13</v>
       </c>
@@ -2287,8 +2112,47 @@
       <c r="I33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="N33" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>1</v>
+      </c>
+      <c r="P33" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>3</v>
+      </c>
+      <c r="R33" t="s">
+        <v>4</v>
+      </c>
+      <c r="S33" t="s">
+        <v>5</v>
+      </c>
+      <c r="T33" t="s">
+        <v>9</v>
+      </c>
+      <c r="U33" t="s">
+        <v>10</v>
+      </c>
+      <c r="V33" t="s">
+        <v>11</v>
+      </c>
+      <c r="W33" t="s">
+        <v>12</v>
+      </c>
+      <c r="X33" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
         <v>4</v>
       </c>
@@ -2309,7 +2173,7 @@
         <v>33.125534119552725</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:26" x14ac:dyDescent="0.3">
       <c r="F35">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
         <v>1.3191169154758013</v>
@@ -2327,7 +2191,7 @@
         <v>3.8898742674058817</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:26" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>13</v>
       </c>
@@ -2341,7 +2205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:26" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
         <v>5</v>
       </c>
@@ -2362,7 +2226,7 @@
         <v>65.855027108862018</v>
       </c>
     </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:26" x14ac:dyDescent="0.3">
       <c r="G39">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
         <v>1.9333402185008477</v>
@@ -2380,7 +2244,7 @@
         <v>3.0412466507963063</v>
       </c>
     </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:26" x14ac:dyDescent="0.3">
       <c r="H41" t="s">
         <v>13</v>
       </c>
@@ -2394,7 +2258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:26" x14ac:dyDescent="0.3">
       <c r="G42" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2279,7 @@
         <v>0.42947289947291256</v>
       </c>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:26" x14ac:dyDescent="0.3">
       <c r="H43">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
         <v>0.53870474088573417</v>
@@ -2433,7 +2297,7 @@
         <v>0.17751313585658005</v>
       </c>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:26" x14ac:dyDescent="0.3">
       <c r="I45" t="s">
         <v>13</v>
       </c>
@@ -2447,7 +2311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:26" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
         <v>10</v>
       </c>
@@ -2468,7 +2332,7 @@
         <v>1.6809206770537894</v>
       </c>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:26" x14ac:dyDescent="0.3">
       <c r="I47">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
         <v>2.5557803975796412E-3</v>
@@ -2752,8 +2616,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N17:Z32">
-    <cfRule type="notContainsText" dxfId="0" priority="1" operator="notContains" text="Ok">
+  <conditionalFormatting sqref="N17:W32">
+    <cfRule type="notContainsText" dxfId="1" priority="1" operator="notContains" text="Ok">
       <formula>ISERROR(SEARCH("Ok",N17))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding all the new images with the fits from the hyperpolarized toolbox
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AE69C8-C3E4-41C2-BE3B-F96509230825}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C21686-B458-4A94-AF09-15EAB84B143F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,28 +130,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -472,7 +451,7 @@
   <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection sqref="A1:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2775,7 +2754,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N17:W32">
-    <cfRule type="notContainsText" dxfId="1" priority="4" operator="notContains" text="Ok">
+    <cfRule type="notContainsText" dxfId="0" priority="4" operator="notContains" text="Ok">
       <formula>ISERROR(SEARCH("Ok",N17))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Getting rid of HW files
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34168D1-DD8F-422C-BD06-D776C9ED798C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC059F3-7718-4E3C-BA36-3165879AAE0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,6 +149,1877 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$B$19:$E$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.2118466964478522E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.2946617313018246E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.5838168193029416E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.9678907413511688E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$B$19:$E$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.2118466964478522E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.2946617313018246E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.5838168193029416E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.9678907413511688E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK + DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.8022337945321011E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.881363600084706E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6168118403753497E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7914781070492852E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C98D-4292-8C4E-2B7EA950A520}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="536602040"/>
+        <c:axId val="536601056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="536602040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536601056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="536601056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536602040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$23:$F$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.11093798793100179</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.4306607486337189E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13975993207811596</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.22335421008885226</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$23:$F$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.11093798793100179</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.4306607486337189E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13975993207811596</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.22335421008885226</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$F$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK + DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.58083466364087666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9743881286951358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64293711066939185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54531597182717306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-01F2-4E3D-A669-2EA217E533B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="303917064"/>
+        <c:axId val="397073928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="303917064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397073928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397073928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="303917064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21F5171-6A3C-46AA-8744-E284A0A3B430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73D92116-571C-49B0-A789-356F3AB2A79B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,7 +2322,7 @@
   <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P16"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2796,5 +4667,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got a little bit better results after introducing R1P and R1Lex as not fixed
</commit_message>
<xml_diff>
--- a/Lacex_summary_hptoolbox.xlsx
+++ b/Lacex_summary_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BAEBF-C99D-4DAD-AF86-0FE520CB4CD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3A492C-1777-49A5-BC13-63A5F4DE91D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{4027078A-84B0-4F52-96FB-34C97BB031FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2321,8 +2321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF99BAD5-59DB-4CD8-989F-B83D7F3C1D42}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>